<commit_message>
Add translation settings to ODK-X forms
</commit_message>
<xml_diff>
--- a/odkx/forms/hh_death.xlsx
+++ b/odkx/forms/hh_death.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -155,6 +155,21 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
+    <t xml:space="preserve">display.title.text.pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.title.text.sw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.locale.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.locale.text.pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.locale.text.sw</t>
+  </si>
+  <si>
     <t xml:space="preserve">form_id</t>
   </si>
   <si>
@@ -174,6 +189,24 @@
   </si>
   <si>
     <t xml:space="preserve">instance_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Português</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiswahili</t>
   </si>
 </sst>
 </file>
@@ -276,7 +309,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
@@ -322,17 +355,17 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,7 +507,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.39"/>
@@ -536,9 +569,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.39"/>
   </cols>
   <sheetData>
@@ -622,17 +655,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,18 +681,33 @@
       <c r="C1" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20210128001</v>
@@ -664,26 +715,74 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>